<commit_message>
Import dữ liệu vào bảng b01, b02, b04 thành công
</commit_message>
<xml_diff>
--- a/TaiLieu/240925/B01.00 Sử dụng dự toán chi KCB tại các tỉnh, TP (tháng 1-8-2023).xlsx
+++ b/TaiLieu/240925/B01.00 Sử dụng dự toán chi KCB tại các tỉnh, TP (tháng 1-8-2023).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\TaiLieu\240925\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E7227A-0945-4DCB-9EB4-6E50880F3E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392253B2-C21E-448E-8A19-7743AB737A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="2445" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -707,7 +707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:T4"/>
     </sheetView>
   </sheetViews>
@@ -780,68 +780,6 @@
       </c>
       <c r="D3" s="2">
         <v>2023</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4">
-        <v>9</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>11</v>
-      </c>
-      <c r="M4">
-        <v>12</v>
-      </c>
-      <c r="N4">
-        <v>13</v>
-      </c>
-      <c r="O4">
-        <v>14</v>
-      </c>
-      <c r="P4">
-        <v>15</v>
-      </c>
-      <c r="Q4">
-        <v>16</v>
-      </c>
-      <c r="R4">
-        <v>17</v>
-      </c>
-      <c r="S4">
-        <v>18</v>
-      </c>
-      <c r="T4">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>